<commit_message>
Changed the Enermerated and mesured events to reflect proper values.
Changed the title of the files to reflect the time delay that is
added to the normal event delay. Corrected events that required a
measured value to activate the event. IE. flat battery.
</commit_message>
<xml_diff>
--- a/Tools/LIFEnet/NXL_Measure_scenario_002.xlsx
+++ b/Tools/LIFEnet/NXL_Measure_scenario_002.xlsx
@@ -1474,8 +1474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89:H132"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1588,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1626,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1664,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1702,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1740,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1778,7 +1779,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1816,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1854,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1892,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1930,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1968,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2003,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -2038,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -2073,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -2111,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -2149,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2187,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -2225,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -2263,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2301,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2339,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2377,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2415,7 +2416,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2453,7 +2454,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2491,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2529,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2567,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2605,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2643,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2681,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2719,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2757,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2795,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2830,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -2865,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -2900,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2938,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -2976,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -3014,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -3052,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -3090,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -3125,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J44">
         <v>1</v>
@@ -3160,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J45">
         <v>1</v>
@@ -3195,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J46" s="22">
         <v>1</v>
@@ -3233,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J47" s="22">
         <v>1</v>
@@ -3271,7 +3272,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J48" s="22">
         <v>1</v>
@@ -3309,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J49" s="22">
         <v>1</v>
@@ -3347,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J50" s="22">
         <v>1</v>
@@ -3385,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J51" s="22">
         <v>1</v>
@@ -3423,7 +3424,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J52" s="22">
         <v>1</v>
@@ -3461,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J53" s="22">
         <v>1</v>
@@ -3499,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J54" s="22">
         <v>1</v>
@@ -3537,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J55" s="22">
         <v>1</v>
@@ -3575,7 +3576,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J56" s="22">
         <v>1</v>
@@ -3611,7 +3612,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J57" s="22">
         <v>1</v>
@@ -3647,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J58" s="22">
         <v>1</v>
@@ -3683,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J59" s="22">
         <v>1</v>
@@ -3721,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J60" s="22">
         <v>1</v>
@@ -3759,7 +3760,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J61" s="22">
         <v>1</v>
@@ -3797,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J62" s="22">
         <v>1</v>
@@ -3835,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J63" s="22">
         <v>1</v>
@@ -3873,7 +3874,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J64" s="22">
         <v>1</v>
@@ -3911,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J65" s="22">
         <v>1</v>
@@ -3949,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J66" s="22">
         <v>1</v>
@@ -3987,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J67" s="22">
         <v>1</v>
@@ -4025,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J68" s="22">
         <v>1</v>
@@ -4063,7 +4064,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J69" s="22">
         <v>1</v>
@@ -4101,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J70" s="22">
         <v>1</v>
@@ -4139,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="I71" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J71" s="22">
         <v>1</v>
@@ -4177,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="I72" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J72" s="22">
         <v>1</v>
@@ -4215,7 +4216,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J73" s="22">
         <v>1</v>
@@ -4253,7 +4254,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J74" s="22">
         <v>1</v>
@@ -4291,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J75" s="22">
         <v>1</v>
@@ -4329,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="I76" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J76" s="22">
         <v>1</v>
@@ -4367,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J77" s="22">
         <v>1</v>
@@ -4405,7 +4406,7 @@
         <v>0</v>
       </c>
       <c r="I78" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J78" s="22">
         <v>1</v>
@@ -4441,7 +4442,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J79" s="22">
         <v>1</v>
@@ -4477,7 +4478,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J80" s="22">
         <v>1</v>
@@ -4513,7 +4514,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J81" s="22">
         <v>1</v>
@@ -4551,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J82" s="22">
         <v>1</v>
@@ -4589,7 +4590,7 @@
         <v>0</v>
       </c>
       <c r="I83" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J83" s="22">
         <v>1</v>
@@ -4627,7 +4628,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J84" s="22">
         <v>1</v>
@@ -4665,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="I85" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J85" s="22">
         <v>1</v>
@@ -4703,7 +4704,7 @@
         <v>0</v>
       </c>
       <c r="I86" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J86" s="22">
         <v>1</v>
@@ -4739,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J87" s="22">
         <v>1</v>
@@ -4775,7 +4776,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="13">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="J88" s="22">
         <v>1</v>

</xml_diff>